<commit_message>
Add RFE-based bulbar regression and update results
Introduced src_analisi/Bulbar_completo_rfe.py for bulbar regression using RFE and LOO, replacing Bulbar_completo.py. Updated and added multiple results Excel files for speech and swallowing RFE analyses, and removed obsolete results. Also updated metrics field names from 'Validation' to 'F1 train' in several speech analysis scripts for consistency.
</commit_message>
<xml_diff>
--- a/Results/RFE/Speech/MFCCs/speech_rfe.xlsx
+++ b/Results/RFE/Speech/MFCCs/speech_rfe.xlsx
@@ -506,7 +506,7 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Validation</t>
+          <t>F1 train</t>
         </is>
       </c>
     </row>
@@ -562,7 +562,7 @@
         <v>0.6</v>
       </c>
       <c r="O2" t="n">
-        <v>0.8177777777777779</v>
+        <v>0.810126582278481</v>
       </c>
     </row>
     <row r="3">
@@ -617,7 +617,7 @@
         <v>0.9</v>
       </c>
       <c r="O3" t="n">
-        <v>0.7622588522588523</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -672,7 +672,7 @@
         <v>0.8</v>
       </c>
       <c r="O4" t="n">
-        <v>0.8254201680672267</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -727,7 +727,7 @@
         <v>0.8</v>
       </c>
       <c r="O5" t="n">
-        <v>0.7636382623224729</v>
+        <v>0.8831168831168831</v>
       </c>
     </row>
     <row r="6">
@@ -743,7 +743,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'activation': 'tanh', 'alpha': 0.0001, 'hidden_layer_sizes': (16, 8), 'learning_rate': 'constant'}</t>
+          <t>{'activation': 'tanh', 'alpha': 0.0001, 'hidden_layer_sizes': (64, 32), 'learning_rate': 'constant'}</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -752,37 +752,37 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" t="n">
         <v>7</v>
       </c>
-      <c r="G6" t="n">
-        <v>3</v>
-      </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I6" t="n">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="J6" t="n">
-        <v>0.6923076923076923</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="L6" t="n">
-        <v>0.5625</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="M6" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="N6" t="n">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="O6" t="n">
-        <v>0.7071467671736886</v>
+        <v>0.6052631578947368</v>
       </c>
     </row>
     <row r="7">
@@ -837,7 +837,7 @@
         <v>0.5</v>
       </c>
       <c r="O7" t="n">
-        <v>0.9866666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -892,7 +892,7 @@
         <v>0.6</v>
       </c>
       <c r="O8" t="n">
-        <v>0.7631746031746032</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -947,7 +947,7 @@
         <v>0.7</v>
       </c>
       <c r="O9" t="n">
-        <v>0.8360784313725491</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1002,7 +1002,7 @@
         <v>0.6</v>
       </c>
       <c r="O10" t="n">
-        <v>0.8831372549019608</v>
+        <v>0.918918918918919</v>
       </c>
     </row>
     <row r="11">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'activation': 'tanh', 'alpha': 0.0001, 'hidden_layer_sizes': (32,), 'learning_rate': 'constant'}</t>
+          <t>{'activation': 'relu', 'alpha': 0.0001, 'hidden_layer_sizes': (64, 32), 'learning_rate': 'constant'}</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>4</v>
@@ -1036,28 +1036,28 @@
         <v>6</v>
       </c>
       <c r="H11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I11" t="n">
-        <v>0.6</v>
+        <v>0.55</v>
       </c>
       <c r="J11" t="n">
-        <v>0.6</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="K11" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="L11" t="n">
-        <v>0.6</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="M11" t="n">
         <v>0.6</v>
       </c>
       <c r="N11" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="O11" t="n">
-        <v>0.6375867269984917</v>
+        <v>0.9333333333333333</v>
       </c>
     </row>
     <row r="12">
@@ -1112,7 +1112,7 @@
         <v>0.5</v>
       </c>
       <c r="O12" t="n">
-        <v>0.9866666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -1167,7 +1167,7 @@
         <v>0.7</v>
       </c>
       <c r="O13" t="n">
-        <v>0.7620881079704609</v>
+        <v>0.9866666666666667</v>
       </c>
     </row>
     <row r="14">
@@ -1222,7 +1222,7 @@
         <v>0.8</v>
       </c>
       <c r="O14" t="n">
-        <v>0.8594444444444445</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -1277,7 +1277,7 @@
         <v>0.5</v>
       </c>
       <c r="O15" t="n">
-        <v>0.8166666666666668</v>
+        <v>0.7733333333333333</v>
       </c>
     </row>
     <row r="16">
@@ -1332,7 +1332,7 @@
         <v>0.5</v>
       </c>
       <c r="O16" t="n">
-        <v>0.617063492063492</v>
+        <v>0.8051948051948052</v>
       </c>
     </row>
   </sheetData>

</xml_diff>